<commit_message>
Started with oops in java
</commit_message>
<xml_diff>
--- a/ADAPT Trackshet.xlsx
+++ b/ADAPT Trackshet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a713729cc1ec1186/ADAPT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="8_{CFE9C939-C390-44C2-B6FC-51DB14D2CAF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0A587AE0-DE71-4EC0-9009-9A619A8D52FD}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="8_{CFE9C939-C390-44C2-B6FC-51DB14D2CAF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{442682ED-2614-4B39-B504-4C4081F664CF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E04EA808-65BC-481F-82D9-8E9E4CE99AC0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t xml:space="preserve">Learnt about UML data diagrams, created repository in github and updated </t>
+  </si>
+  <si>
+    <t>Download and Installation of JDK, added path and coded basic programs</t>
+  </si>
+  <si>
+    <t>7PM-9PM</t>
+  </si>
+  <si>
+    <t>Started with OOPS concept in JAVA</t>
   </si>
 </sst>
 </file>
@@ -116,8 +125,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="167" formatCode="[$-F400]h\.mm\.ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h\.mm\.ss\ AM/PM"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -159,10 +168,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -211,15 +220,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9BB3EA3-22B6-4D96-BD5E-C5981102B7C0}" name="Table1" displayName="Table1" ref="B1:G29" totalsRowShown="0" headerRowDxfId="7" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9BB3EA3-22B6-4D96-BD5E-C5981102B7C0}" name="Table1" displayName="Table1" ref="B1:G29" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="B1:G29" xr:uid="{98C3C62C-FACF-4506-B032-2D6F0DE489AF}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{9C5323C0-40F5-4853-8FB5-26DE70D7462E}" name="Date" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{FA26433C-5C8E-431D-AB49-C0E645DF4C53}" name="Time" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{0FBDE0EC-4347-43BA-A12F-920616DC0F1F}" name="Topic" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{524C6483-830C-49F4-B22F-FCFD970FD9A2}" name="Description" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{71C8D5C7-1E2D-4E3F-9F49-27E9D89D7726}" name="Github Link " dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{A709E9A6-F691-4076-BD91-3A374CA03E25}" name="Mentor's Review" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{9C5323C0-40F5-4853-8FB5-26DE70D7462E}" name="Date" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{FA26433C-5C8E-431D-AB49-C0E645DF4C53}" name="Time" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{0FBDE0EC-4347-43BA-A12F-920616DC0F1F}" name="Topic" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{524C6483-830C-49F4-B22F-FCFD970FD9A2}" name="Description" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{71C8D5C7-1E2D-4E3F-9F49-27E9D89D7726}" name="Github Link " dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{A709E9A6-F691-4076-BD91-3A374CA03E25}" name="Mentor's Review" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -525,7 +534,7 @@
   <dimension ref="B1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -751,18 +760,34 @@
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="B14" s="4">
+        <v>44212</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="B15" s="4">
+        <v>44212</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>

</xml_diff>

<commit_message>
Done Assignment-1 in Core Java
</commit_message>
<xml_diff>
--- a/ADAPT Trackshet.xlsx
+++ b/ADAPT Trackshet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a713729cc1ec1186/ADAPT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="8_{CFE9C939-C390-44C2-B6FC-51DB14D2CAF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{442682ED-2614-4B39-B504-4C4081F664CF}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="8_{CFE9C939-C390-44C2-B6FC-51DB14D2CAF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4D33403B-9897-44BC-9E89-883AAA41C87A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E04EA808-65BC-481F-82D9-8E9E4CE99AC0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -118,6 +118,15 @@
   </si>
   <si>
     <t>Started with OOPS concept in JAVA</t>
+  </si>
+  <si>
+    <t>Done Assignment 1 In Java</t>
+  </si>
+  <si>
+    <t>Building OOPS Application in JAVA</t>
+  </si>
+  <si>
+    <t>1PM-10PM</t>
   </si>
 </sst>
 </file>
@@ -534,7 +543,7 @@
   <dimension ref="B1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -792,18 +801,34 @@
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="B16" s="4">
+        <v>44214</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="B17" s="4">
+        <v>44214</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>

</xml_diff>

<commit_message>
Started Assignment of Collections
</commit_message>
<xml_diff>
--- a/ADAPT Trackshet.xlsx
+++ b/ADAPT Trackshet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a713729cc1ec1186/ADAPT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="8_{CFE9C939-C390-44C2-B6FC-51DB14D2CAF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4D33403B-9897-44BC-9E89-883AAA41C87A}"/>
+  <xr:revisionPtr revIDLastSave="205" documentId="8_{CFE9C939-C390-44C2-B6FC-51DB14D2CAF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C3871993-2813-4A57-9D84-D75299423A17}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E04EA808-65BC-481F-82D9-8E9E4CE99AC0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -123,10 +123,31 @@
     <t>Done Assignment 1 In Java</t>
   </si>
   <si>
-    <t>Building OOPS Application in JAVA</t>
-  </si>
-  <si>
     <t>1PM-10PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Building OOPS Application in JAVA</t>
+  </si>
+  <si>
+    <t>Started with Exception Handling in Java</t>
+  </si>
+  <si>
+    <t>Practice on Exception Handling</t>
+  </si>
+  <si>
+    <t>Full Day</t>
+  </si>
+  <si>
+    <t>Done Assignment 2 In Java(1-5 Questions)</t>
+  </si>
+  <si>
+    <t>Started with Collections</t>
+  </si>
+  <si>
+    <t>Completed Assignment 2 - Intermediate OOPS Assignment</t>
+  </si>
+  <si>
+    <t>Done Assignment 3 - Collection Framework Assignment</t>
   </si>
 </sst>
 </file>
@@ -229,8 +250,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9BB3EA3-22B6-4D96-BD5E-C5981102B7C0}" name="Table1" displayName="Table1" ref="B1:G29" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G29" xr:uid="{98C3C62C-FACF-4506-B032-2D6F0DE489AF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9BB3EA3-22B6-4D96-BD5E-C5981102B7C0}" name="Table1" displayName="Table1" ref="B1:G31" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G31" xr:uid="{98C3C62C-FACF-4506-B032-2D6F0DE489AF}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9C5323C0-40F5-4853-8FB5-26DE70D7462E}" name="Date" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{FA26433C-5C8E-431D-AB49-C0E645DF4C53}" name="Time" dataDxfId="4"/>
@@ -540,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B23A41-ACA0-448D-9248-84323645C9D0}">
-  <dimension ref="B1:G29"/>
+  <dimension ref="B1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -821,62 +842,110 @@
         <v>44214</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="B18" s="4">
+        <v>44215</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="B19" s="4">
+        <v>44216</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="B20" s="4">
+        <v>44217</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="B21" s="4">
+        <v>44218</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="B22" s="4">
+        <v>44218</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="B23" s="4">
+        <v>44219</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
@@ -928,6 +997,22 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>